<commit_message>
Rework documentation info in excel file
</commit_message>
<xml_diff>
--- a/DataValueClustering/experiments/exports/study/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210401-085923_final.xlsx
+++ b/DataValueClustering/experiments/exports/study/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210401-085923_final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viola Wenz\Documents\Repositories\data-value-clustering\DataValueClustering\experiments\exports\evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viola Wenz\Documents\Repositories\data-value-clustering\DataValueClustering\experiments\exports\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster_Original" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="158">
   <si>
     <t>#original</t>
   </si>
@@ -362,13 +362,148 @@
   </si>
   <si>
     <t>Terminologie Empfehlung</t>
+  </si>
+  <si>
+    <t>&lt;xs:complexType name="actorInRoleComplexType" id="actorInRoleComplexType"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:annotation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:documentation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="description"&gt;Contains actor information with role, attribution and</t>
+  </si>
+  <si>
+    <t>extent, where applicable, related to the event the actor participated in or was</t>
+  </si>
+  <si>
+    <t>present at.&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="furtherReading"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ref target="https://www.getty.edu/research/publications/electronic_publications/cdwa/14creation.html#Creator-Role"&gt;</t>
+  </si>
+  <si>
+    <t>CDWA: 4.1.4. Creator Role&lt;/tei:ref&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="dataValues"&gt;Not applicable&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:documentation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:annotation&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:sequence&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:element name="actor" type="lido:actorComplexType" id="actor_actorInRoleComplexType"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:element&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:element name="roleActor" minOccurs="0" maxOccurs="unbounded" id="roleActor"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:element name="attributionQualifierActor" type="lido:conceptMixedComplexType"</t>
+  </si>
+  <si>
+    <t>minOccurs="0" maxOccurs="unbounded" id="attributionQualifierActor"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="description"&gt;An index element qualifying the attribution of an</t>
+  </si>
+  <si>
+    <t>actor; applicable when the attribution is uncertain or in dispute, when</t>
+  </si>
+  <si>
+    <t>there is more than one actor, or when the attribution otherwise requires</t>
+  </si>
+  <si>
+    <t>explanation.&lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>Examples may include &lt;em&gt;attributed to&lt;/em&gt;, &lt;em&gt;studio of&lt;/em&gt;, or &lt;em&gt;style</t>
+  </si>
+  <si>
+    <t>of&lt;/em&gt;.&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="label"&gt;Attribution Qualifier Actor&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ref target="https://www.getty.edu/research/publications/electronic_publications/cdwa/14creation.html#Qualifier"&gt;</t>
+  </si>
+  <si>
+    <t>CDWA: 4.1.2. Creator Qualifier&lt;/tei:ref&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="dataValues"&gt;Controlled terminology&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tei:ab type="recommendation"&gt;Linked open vocabulary for</t>
+  </si>
+  <si>
+    <t>&lt;tei:ref target="accompanying-document.html#attributionQualifierActor"&gt;Attribution Qualifier Actor&lt;/tei:ref&gt;&lt;/tei:ab&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:appinfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sch:pattern&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sch:rule context="lido:attributionQualifierActor"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sch:extends rule="sch_MixedContent"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sch:extends rule="sch_MixedContentInfo"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sch:extends rule="sch_SKOS"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/sch:rule&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/sch:pattern&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:appinfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:element name="extentActor" type="lido:conceptMixedComplexType" minOccurs="0"</t>
+  </si>
+  <si>
+    <t>maxOccurs="unbounded" id="extentActor"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xs:element name="sourceActorInRole" type="lido:textComplexType" minOccurs="0" maxOccurs="unbounded" id="sourceActorInRole"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:sequence&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xs:complexType&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +531,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -568,6 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3309,8 +3453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y84"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4163,7 +4307,7 @@
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D50" s="13"/>
@@ -5053,16 +5197,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5091,6 +5236,1305 @@
         <v>111</v>
       </c>
     </row>
+    <row r="76" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B77" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="11"/>
+    </row>
+    <row r="78" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="18"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
+      <c r="O78" s="13"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="14"/>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B79" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
+      <c r="O79" s="13"/>
+      <c r="P79" s="13"/>
+      <c r="Q79" s="13"/>
+      <c r="R79" s="14"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B80" s="12"/>
+      <c r="C80" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="13"/>
+      <c r="N80" s="13"/>
+      <c r="O80" s="13"/>
+      <c r="P80" s="13"/>
+      <c r="Q80" s="13"/>
+      <c r="R80" s="14"/>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B81" s="12"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
+      <c r="O81" s="13"/>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="13"/>
+      <c r="R81" s="14"/>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B82" s="12"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="13"/>
+      <c r="R82" s="14"/>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B83" s="12"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
+      <c r="O83" s="13"/>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="13"/>
+      <c r="R83" s="14"/>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B84" s="12"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13"/>
+      <c r="O84" s="13"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="13"/>
+      <c r="R84" s="14"/>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B85" s="12"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="13"/>
+      <c r="R85" s="14"/>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B86" s="12"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="13"/>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="14"/>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B87" s="12"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="13"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="13"/>
+      <c r="P87" s="13"/>
+      <c r="Q87" s="13"/>
+      <c r="R87" s="14"/>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B88" s="12"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="13"/>
+      <c r="P88" s="13"/>
+      <c r="Q88" s="13"/>
+      <c r="R88" s="14"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B89" s="12"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="13"/>
+      <c r="N89" s="13"/>
+      <c r="O89" s="13"/>
+      <c r="P89" s="13"/>
+      <c r="Q89" s="13"/>
+      <c r="R89" s="14"/>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B90" s="12"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="13"/>
+      <c r="N90" s="13"/>
+      <c r="O90" s="13"/>
+      <c r="P90" s="13"/>
+      <c r="Q90" s="13"/>
+      <c r="R90" s="14"/>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B91" s="12"/>
+      <c r="C91" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="13"/>
+      <c r="N91" s="13"/>
+      <c r="O91" s="13"/>
+      <c r="P91" s="13"/>
+      <c r="Q91" s="13"/>
+      <c r="R91" s="14"/>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B92" s="12"/>
+      <c r="C92" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="13"/>
+      <c r="N92" s="13"/>
+      <c r="O92" s="13"/>
+      <c r="P92" s="13"/>
+      <c r="Q92" s="13"/>
+      <c r="R92" s="14"/>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B93" s="12"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="13"/>
+      <c r="N93" s="13"/>
+      <c r="O93" s="13"/>
+      <c r="P93" s="13"/>
+      <c r="Q93" s="13"/>
+      <c r="R93" s="14"/>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B94" s="12"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="13"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="13"/>
+      <c r="P94" s="13"/>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="14"/>
+    </row>
+    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B95" s="12"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
+      <c r="M95" s="13"/>
+      <c r="N95" s="13"/>
+      <c r="O95" s="13"/>
+      <c r="P95" s="13"/>
+      <c r="Q95" s="13"/>
+      <c r="R95" s="14"/>
+    </row>
+    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B96" s="12"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="13"/>
+      <c r="N96" s="13"/>
+      <c r="O96" s="13"/>
+      <c r="P96" s="13"/>
+      <c r="Q96" s="13"/>
+      <c r="R96" s="14"/>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B97" s="12"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+      <c r="M97" s="13"/>
+      <c r="N97" s="13"/>
+      <c r="O97" s="13"/>
+      <c r="P97" s="13"/>
+      <c r="Q97" s="13"/>
+      <c r="R97" s="14"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="12"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="13"/>
+      <c r="N98" s="13"/>
+      <c r="O98" s="13"/>
+      <c r="P98" s="13"/>
+      <c r="Q98" s="13"/>
+      <c r="R98" s="14"/>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B99" s="12"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="13"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="13"/>
+      <c r="P99" s="13"/>
+      <c r="Q99" s="13"/>
+      <c r="R99" s="14"/>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="12"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13"/>
+      <c r="N100" s="13"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="13"/>
+      <c r="Q100" s="13"/>
+      <c r="R100" s="14"/>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B101" s="12"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="13"/>
+      <c r="M101" s="13"/>
+      <c r="N101" s="13"/>
+      <c r="O101" s="13"/>
+      <c r="P101" s="13"/>
+      <c r="Q101" s="13"/>
+      <c r="R101" s="14"/>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B102" s="12"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
+      <c r="M102" s="13"/>
+      <c r="N102" s="13"/>
+      <c r="O102" s="13"/>
+      <c r="P102" s="13"/>
+      <c r="Q102" s="13"/>
+      <c r="R102" s="14"/>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B103" s="12"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+      <c r="M103" s="13"/>
+      <c r="N103" s="13"/>
+      <c r="O103" s="13"/>
+      <c r="P103" s="13"/>
+      <c r="Q103" s="13"/>
+      <c r="R103" s="14"/>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B104" s="12"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13"/>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
+      <c r="M104" s="13"/>
+      <c r="N104" s="13"/>
+      <c r="O104" s="13"/>
+      <c r="P104" s="13"/>
+      <c r="Q104" s="13"/>
+      <c r="R104" s="14"/>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B105" s="12"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I105" s="13"/>
+      <c r="J105" s="13"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
+      <c r="M105" s="13"/>
+      <c r="N105" s="13"/>
+      <c r="O105" s="13"/>
+      <c r="P105" s="13"/>
+      <c r="Q105" s="13"/>
+      <c r="R105" s="14"/>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B106" s="12"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I106" s="13"/>
+      <c r="J106" s="13"/>
+      <c r="K106" s="13"/>
+      <c r="L106" s="13"/>
+      <c r="M106" s="13"/>
+      <c r="N106" s="13"/>
+      <c r="O106" s="13"/>
+      <c r="P106" s="13"/>
+      <c r="Q106" s="13"/>
+      <c r="R106" s="14"/>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B107" s="12"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I107" s="13"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
+      <c r="M107" s="13"/>
+      <c r="N107" s="13"/>
+      <c r="O107" s="13"/>
+      <c r="P107" s="13"/>
+      <c r="Q107" s="13"/>
+      <c r="R107" s="14"/>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B108" s="12"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+      <c r="M108" s="13"/>
+      <c r="N108" s="13"/>
+      <c r="O108" s="13"/>
+      <c r="P108" s="13"/>
+      <c r="Q108" s="13"/>
+      <c r="R108" s="14"/>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B109" s="12"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="13"/>
+      <c r="K109" s="13"/>
+      <c r="L109" s="13"/>
+      <c r="M109" s="13"/>
+      <c r="N109" s="13"/>
+      <c r="O109" s="13"/>
+      <c r="P109" s="13"/>
+      <c r="Q109" s="13"/>
+      <c r="R109" s="14"/>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B110" s="12"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="13"/>
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
+      <c r="M110" s="13"/>
+      <c r="N110" s="13"/>
+      <c r="O110" s="13"/>
+      <c r="P110" s="13"/>
+      <c r="Q110" s="13"/>
+      <c r="R110" s="14"/>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B111" s="12"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I111" s="13"/>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
+      <c r="M111" s="13"/>
+      <c r="N111" s="13"/>
+      <c r="O111" s="13"/>
+      <c r="P111" s="13"/>
+      <c r="Q111" s="13"/>
+      <c r="R111" s="14"/>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B112" s="12"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J112" s="13"/>
+      <c r="K112" s="13"/>
+      <c r="L112" s="13"/>
+      <c r="M112" s="13"/>
+      <c r="N112" s="13"/>
+      <c r="O112" s="13"/>
+      <c r="P112" s="13"/>
+      <c r="Q112" s="13"/>
+      <c r="R112" s="14"/>
+    </row>
+    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B113" s="12"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="13"/>
+      <c r="K113" s="13"/>
+      <c r="L113" s="13"/>
+      <c r="M113" s="13"/>
+      <c r="N113" s="13"/>
+      <c r="O113" s="13"/>
+      <c r="P113" s="13"/>
+      <c r="Q113" s="13"/>
+      <c r="R113" s="14"/>
+    </row>
+    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B114" s="12"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="13"/>
+      <c r="K114" s="13"/>
+      <c r="L114" s="13"/>
+      <c r="M114" s="13"/>
+      <c r="N114" s="13"/>
+      <c r="O114" s="13"/>
+      <c r="P114" s="13"/>
+      <c r="Q114" s="13"/>
+      <c r="R114" s="14"/>
+    </row>
+    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B115" s="12"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="13"/>
+      <c r="K115" s="13"/>
+      <c r="L115" s="13"/>
+      <c r="M115" s="13"/>
+      <c r="N115" s="13"/>
+      <c r="O115" s="13"/>
+      <c r="P115" s="13"/>
+      <c r="Q115" s="13"/>
+      <c r="R115" s="14"/>
+    </row>
+    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B116" s="12"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+      <c r="M116" s="13"/>
+      <c r="N116" s="13"/>
+      <c r="O116" s="13"/>
+      <c r="P116" s="13"/>
+      <c r="Q116" s="13"/>
+      <c r="R116" s="14"/>
+    </row>
+    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B117" s="12"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="13"/>
+      <c r="K117" s="13"/>
+      <c r="L117" s="13"/>
+      <c r="M117" s="13"/>
+      <c r="N117" s="13"/>
+      <c r="O117" s="13"/>
+      <c r="P117" s="13"/>
+      <c r="Q117" s="13"/>
+      <c r="R117" s="14"/>
+    </row>
+    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B118" s="12"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="13"/>
+      <c r="K118" s="13"/>
+      <c r="L118" s="13"/>
+      <c r="M118" s="13"/>
+      <c r="N118" s="13"/>
+      <c r="O118" s="13"/>
+      <c r="P118" s="13"/>
+      <c r="Q118" s="13"/>
+      <c r="R118" s="14"/>
+    </row>
+    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B119" s="12"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="13"/>
+      <c r="K119" s="13"/>
+      <c r="L119" s="13"/>
+      <c r="M119" s="13"/>
+      <c r="N119" s="13"/>
+      <c r="O119" s="13"/>
+      <c r="P119" s="13"/>
+      <c r="Q119" s="13"/>
+      <c r="R119" s="14"/>
+    </row>
+    <row r="120" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B120" s="12"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="I120" s="13"/>
+      <c r="J120" s="13"/>
+      <c r="K120" s="13"/>
+      <c r="L120" s="13"/>
+      <c r="M120" s="13"/>
+      <c r="N120" s="13"/>
+      <c r="O120" s="13"/>
+      <c r="P120" s="13"/>
+      <c r="Q120" s="13"/>
+      <c r="R120" s="14"/>
+    </row>
+    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B121" s="12"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="13"/>
+      <c r="M121" s="13"/>
+      <c r="N121" s="13"/>
+      <c r="O121" s="13"/>
+      <c r="P121" s="13"/>
+      <c r="Q121" s="13"/>
+      <c r="R121" s="14"/>
+    </row>
+    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B122" s="12"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J122" s="13"/>
+      <c r="K122" s="13"/>
+      <c r="L122" s="13"/>
+      <c r="M122" s="13"/>
+      <c r="N122" s="13"/>
+      <c r="O122" s="13"/>
+      <c r="P122" s="13"/>
+      <c r="Q122" s="13"/>
+      <c r="R122" s="14"/>
+    </row>
+    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B123" s="12"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J123" s="13"/>
+      <c r="K123" s="13"/>
+      <c r="L123" s="13"/>
+      <c r="M123" s="13"/>
+      <c r="N123" s="13"/>
+      <c r="O123" s="13"/>
+      <c r="P123" s="13"/>
+      <c r="Q123" s="13"/>
+      <c r="R123" s="14"/>
+    </row>
+    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B124" s="12"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I124" s="13"/>
+      <c r="J124" s="13"/>
+      <c r="K124" s="13"/>
+      <c r="L124" s="13"/>
+      <c r="M124" s="13"/>
+      <c r="N124" s="13"/>
+      <c r="O124" s="13"/>
+      <c r="P124" s="13"/>
+      <c r="Q124" s="13"/>
+      <c r="R124" s="14"/>
+    </row>
+    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B125" s="12"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H125" s="13"/>
+      <c r="I125" s="13"/>
+      <c r="J125" s="13"/>
+      <c r="K125" s="13"/>
+      <c r="L125" s="13"/>
+      <c r="M125" s="13"/>
+      <c r="N125" s="13"/>
+      <c r="O125" s="13"/>
+      <c r="P125" s="13"/>
+      <c r="Q125" s="13"/>
+      <c r="R125" s="14"/>
+    </row>
+    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B126" s="12"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="13"/>
+      <c r="J126" s="13"/>
+      <c r="K126" s="13"/>
+      <c r="L126" s="13"/>
+      <c r="M126" s="13"/>
+      <c r="N126" s="13"/>
+      <c r="O126" s="13"/>
+      <c r="P126" s="13"/>
+      <c r="Q126" s="13"/>
+      <c r="R126" s="14"/>
+    </row>
+    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B127" s="12"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="13"/>
+      <c r="K127" s="13"/>
+      <c r="L127" s="13"/>
+      <c r="M127" s="13"/>
+      <c r="N127" s="13"/>
+      <c r="O127" s="13"/>
+      <c r="P127" s="13"/>
+      <c r="Q127" s="13"/>
+      <c r="R127" s="14"/>
+    </row>
+    <row r="128" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B128" s="12"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="13"/>
+      <c r="K128" s="13"/>
+      <c r="L128" s="13"/>
+      <c r="M128" s="13"/>
+      <c r="N128" s="13"/>
+      <c r="O128" s="13"/>
+      <c r="P128" s="13"/>
+      <c r="Q128" s="13"/>
+      <c r="R128" s="14"/>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B129" s="12"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+      <c r="I129" s="13"/>
+      <c r="J129" s="13"/>
+      <c r="K129" s="13"/>
+      <c r="L129" s="13"/>
+      <c r="M129" s="13"/>
+      <c r="N129" s="13"/>
+      <c r="O129" s="13"/>
+      <c r="P129" s="13"/>
+      <c r="Q129" s="13"/>
+      <c r="R129" s="14"/>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B130" s="12"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="13"/>
+      <c r="J130" s="13"/>
+      <c r="K130" s="13"/>
+      <c r="L130" s="13"/>
+      <c r="M130" s="13"/>
+      <c r="N130" s="13"/>
+      <c r="O130" s="13"/>
+      <c r="P130" s="13"/>
+      <c r="Q130" s="13"/>
+      <c r="R130" s="14"/>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B131" s="12"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="13"/>
+      <c r="K131" s="13"/>
+      <c r="L131" s="13"/>
+      <c r="M131" s="13"/>
+      <c r="N131" s="13"/>
+      <c r="O131" s="13"/>
+      <c r="P131" s="13"/>
+      <c r="Q131" s="13"/>
+      <c r="R131" s="14"/>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B132" s="12"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="13"/>
+      <c r="K132" s="13"/>
+      <c r="L132" s="13"/>
+      <c r="M132" s="13"/>
+      <c r="N132" s="13"/>
+      <c r="O132" s="13"/>
+      <c r="P132" s="13"/>
+      <c r="Q132" s="13"/>
+      <c r="R132" s="14"/>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B133" s="12"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="13"/>
+      <c r="J133" s="13"/>
+      <c r="K133" s="13"/>
+      <c r="L133" s="13"/>
+      <c r="M133" s="13"/>
+      <c r="N133" s="13"/>
+      <c r="O133" s="13"/>
+      <c r="P133" s="13"/>
+      <c r="Q133" s="13"/>
+      <c r="R133" s="14"/>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B134" s="12"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="13"/>
+      <c r="K134" s="13"/>
+      <c r="L134" s="13"/>
+      <c r="M134" s="13"/>
+      <c r="N134" s="13"/>
+      <c r="O134" s="13"/>
+      <c r="P134" s="13"/>
+      <c r="Q134" s="13"/>
+      <c r="R134" s="14"/>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B135" s="12"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="13"/>
+      <c r="K135" s="13"/>
+      <c r="L135" s="13"/>
+      <c r="M135" s="13"/>
+      <c r="N135" s="13"/>
+      <c r="O135" s="13"/>
+      <c r="P135" s="13"/>
+      <c r="Q135" s="13"/>
+      <c r="R135" s="14"/>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B136" s="12"/>
+      <c r="C136" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="13"/>
+      <c r="K136" s="13"/>
+      <c r="L136" s="13"/>
+      <c r="M136" s="13"/>
+      <c r="N136" s="13"/>
+      <c r="O136" s="13"/>
+      <c r="P136" s="13"/>
+      <c r="Q136" s="13"/>
+      <c r="R136" s="14"/>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B137" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="13"/>
+      <c r="K137" s="13"/>
+      <c r="L137" s="13"/>
+      <c r="M137" s="13"/>
+      <c r="N137" s="13"/>
+      <c r="O137" s="13"/>
+      <c r="P137" s="13"/>
+      <c r="Q137" s="13"/>
+      <c r="R137" s="14"/>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B138" s="15"/>
+      <c r="C138" s="16"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
+      <c r="J138" s="16"/>
+      <c r="K138" s="16"/>
+      <c r="L138" s="16"/>
+      <c r="M138" s="16"/>
+      <c r="N138" s="16"/>
+      <c r="O138" s="16"/>
+      <c r="P138" s="16"/>
+      <c r="Q138" s="16"/>
+      <c r="R138" s="17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add documentation to excel files.
</commit_message>
<xml_diff>
--- a/DataValueClustering/experiments/exports/study/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210401-085923_final.xlsx
+++ b/DataValueClustering/experiments/exports/study/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210401-085923_final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viola Wenz\Documents\Repositories\data-value-clustering\DataValueClustering\experiments\exports\study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Arbeit\SourceTree\data-value-clustering\DataValueClustering\experiments\exports\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A168059F-4B54-434F-8C3A-DD06CF76B702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster_Original" sheetId="1" r:id="rId1"/>
@@ -502,7 +503,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -690,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -711,7 +712,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -746,7 +776,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -795,7 +831,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -839,7 +881,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -883,7 +931,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -991,6 +1045,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1026,6 +1097,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1201,7 +1289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1819,7 +1907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:W22"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
@@ -2463,7 +2551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AH23"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
@@ -3450,11 +3538,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,554 +3881,554 @@
       <c r="P22" s="13"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="14"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="22"/>
       <c r="P23" s="13"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="14"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
       <c r="P24" s="13"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="14"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
       <c r="P25" s="13"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="13" t="s">
+      <c r="B26" s="23"/>
+      <c r="C26" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="14"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
       <c r="P26" s="13"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="14"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="22"/>
       <c r="P27" s="13"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="23"/>
+      <c r="C28" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="14"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="22"/>
       <c r="P28" s="13"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="14"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
       <c r="P29" s="13"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="22"/>
       <c r="P30" s="13"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="23"/>
+      <c r="C31" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="14"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="22"/>
       <c r="P31" s="13"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="23"/>
+      <c r="C32" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="14"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="22"/>
       <c r="P32" s="13"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13" t="s">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="14"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="22"/>
       <c r="P33" s="13"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-      <c r="C34" s="13" t="s">
+      <c r="B34" s="23"/>
+      <c r="C34" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="14"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="22"/>
       <c r="P34" s="13"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="23"/>
+      <c r="C35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="14"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="22"/>
       <c r="P35" s="13"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13" t="s">
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="14"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="22"/>
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="23"/>
+      <c r="C37" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="14"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="22"/>
       <c r="P37" s="13"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
-      <c r="C38" s="13" t="s">
+      <c r="B38" s="23"/>
+      <c r="C38" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="14"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="22"/>
       <c r="P38" s="13"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13" t="s">
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="14"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="22"/>
       <c r="P39" s="13"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
-      <c r="C40" s="13" t="s">
+      <c r="B40" s="23"/>
+      <c r="C40" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="14"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="22"/>
       <c r="P40" s="13"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
-      <c r="C41" s="13" t="s">
+      <c r="B41" s="23"/>
+      <c r="C41" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="14"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="22"/>
       <c r="P41" s="13"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="12"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13" t="s">
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="14"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="22"/>
       <c r="P42" s="13"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13" t="s">
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="14"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="22"/>
       <c r="P43" s="13"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
-      <c r="C44" s="13" t="s">
+      <c r="B44" s="23"/>
+      <c r="C44" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="14"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="22"/>
       <c r="P44" s="13"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="12"/>
-      <c r="C45" s="13" t="s">
+      <c r="B45" s="23"/>
+      <c r="C45" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="14"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="22"/>
       <c r="P45" s="13"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="12"/>
-      <c r="C46" s="13" t="s">
+      <c r="B46" s="23"/>
+      <c r="C46" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="14"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="22"/>
       <c r="P46" s="13"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="12"/>
-      <c r="C47" s="13" t="s">
+      <c r="B47" s="23"/>
+      <c r="C47" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="14"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="22"/>
       <c r="P47" s="13"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="12"/>
-      <c r="C48" s="13" t="s">
+      <c r="B48" s="23"/>
+      <c r="C48" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="14"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="22"/>
       <c r="P48" s="13"/>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="23"/>
+      <c r="C49" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="14"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="22"/>
       <c r="P49" s="13"/>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B50" s="12"/>
-      <c r="C50" s="20" t="s">
+      <c r="B50" s="23"/>
+      <c r="C50" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="14"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="26"/>
       <c r="P50" s="13"/>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="17"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="28"/>
+      <c r="O51" s="29"/>
       <c r="P51" s="13"/>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.25">
@@ -5196,6 +5284,37 @@
       <c r="Y84" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B51:O51"/>
+    <mergeCell ref="C45:O45"/>
+    <mergeCell ref="C46:O46"/>
+    <mergeCell ref="C47:O47"/>
+    <mergeCell ref="C48:O48"/>
+    <mergeCell ref="C49:O49"/>
+    <mergeCell ref="C50:O50"/>
+    <mergeCell ref="C40:O40"/>
+    <mergeCell ref="D42:O42"/>
+    <mergeCell ref="C44:O44"/>
+    <mergeCell ref="D39:O39"/>
+    <mergeCell ref="C41:O41"/>
+    <mergeCell ref="D43:O43"/>
+    <mergeCell ref="C34:O34"/>
+    <mergeCell ref="C37:O37"/>
+    <mergeCell ref="D33:O33"/>
+    <mergeCell ref="C35:O35"/>
+    <mergeCell ref="D36:O36"/>
+    <mergeCell ref="C38:O38"/>
+    <mergeCell ref="C28:O28"/>
+    <mergeCell ref="C31:O31"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="C29:O29"/>
+    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="C32:O32"/>
+    <mergeCell ref="C24:O24"/>
+    <mergeCell ref="C25:O25"/>
+    <mergeCell ref="B23:O23"/>
+    <mergeCell ref="C26:O26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5203,10 +5322,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>

</xml_diff>